<commit_message>
feat: delete the sheet that acted as the template
OCD-4438
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
+++ b/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youngto\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2643EC8E-A24A-4347-BE60-896401F1C705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2ED7B8-E882-4576-85A5-A99247CFE756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2820" windowWidth="21600" windowHeight="11280" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="9" r:id="rId1"/>
@@ -254,7 +254,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{86D36E8E-CBD7-4E76-80D3-E7D3607652E4}" type="CELLRANGE">
+                    <a:fld id="{57F99CE6-533B-4D4E-998D-A8413B123192}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr b="1">
@@ -324,7 +324,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34975F00-0731-4181-8809-C032206A80C0}" type="CELLRANGE">
+                    <a:fld id="{1D26D014-8A31-4F0B-A0DC-C3DA8EF536C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -357,7 +357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0FA71812-3991-4DCF-BD26-666908CD29C3}" type="CELLRANGE">
+                    <a:fld id="{38B45843-60E9-46FE-9829-1FAB94696776}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -390,7 +390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5D44BD5-6A64-4FBF-8DA7-D3B955DE8208}" type="CELLRANGE">
+                    <a:fld id="{841C167C-4C11-4E6C-9792-74718E802307}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -423,7 +423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B35FDDA0-095A-4BD4-9A70-D8B9784F07B8}" type="CELLRANGE">
+                    <a:fld id="{04F3B724-FE78-4E14-B78A-56792D49100C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -456,7 +456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{305355AE-1913-4E94-BF2A-47053E8440CB}" type="CELLRANGE">
+                    <a:fld id="{841AB74C-E4F1-4950-A792-086326039016}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -489,7 +489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D9D5BBD-5A3C-4363-933A-26D37098D129}" type="CELLRANGE">
+                    <a:fld id="{22535987-08D2-4187-B55A-3CC46081ADC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -522,7 +522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3EA7AF45-D442-428C-964D-66974125B9B0}" type="CELLRANGE">
+                    <a:fld id="{891C1DB0-42E6-4828-BB55-309048531203}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -555,7 +555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{607EFEE1-CC4F-48D0-801C-BA2CB417BF95}" type="CELLRANGE">
+                    <a:fld id="{A5847E59-7AF4-4303-BD1B-452AA55787E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -588,7 +588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C084D6BC-E1CF-4D5F-8C52-15B7C73B3E04}" type="CELLRANGE">
+                    <a:fld id="{5DC4736F-CB52-4AE4-93F5-7F22FD52FC4E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -621,7 +621,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E675EA8-D164-44EA-85C7-98CDABF22CD7}" type="CELLRANGE">
+                    <a:fld id="{216BC88A-CA91-4712-882C-F11B4D08F6D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -654,7 +654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21AC6DC3-3509-4FE8-9FEE-0EC88448F8AA}" type="CELLRANGE">
+                    <a:fld id="{94A7C9B2-5872-418B-8801-AAB376002193}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2781,7 +2781,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="U5" sqref="U5:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,10 +2982,7 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="U5" s="3">
-        <f>249/257</f>
-        <v>0.9688715953307393</v>
-      </c>
+      <c r="U5" s="3"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3027,10 +3024,7 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="U6" s="3">
-        <f>32/249</f>
-        <v>0.12851405622489959</v>
-      </c>
+      <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3134,23 +3128,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100054B99873F0D6546B559819D0825E003" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cffa56ad5792ecafcd3589bab1bbb308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xmlns:ns4="6c1397f4-a2e4-41e1-a56a-3ef30e67d471" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68c1c6e3f17b441c567360df559ac01a" ns3:_="" ns4:_="">
     <xsd:import namespace="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
@@ -3389,32 +3366,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA91FC1-FB23-421D-B0F5-8B5FD962DF28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3431,4 +3400,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: remove leftover values from template spreadsheet
OCD-4438
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
+++ b/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youngto\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D74D683-94FE-4CF9-BDD4-0933B049E7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE1997E-EF65-4C48-8976-553CBD4EBDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="2145" yWindow="1785" windowWidth="21600" windowHeight="11205" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="11" r:id="rId1"/>
@@ -1876,17 +1876,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F5CA64-B349-4540-8897-9876CE15B639}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1927,7 +1925,7 @@
         <v>45349</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2021,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2062,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2102,12 +2100,9 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="U5" s="3">
-        <f>249/257</f>
-        <v>0.9688715953307393</v>
-      </c>
+      <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2147,12 +2142,9 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="U6" s="3">
-        <f>32/249</f>
-        <v>0.12851405622489959</v>
-      </c>
+      <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2194,7 +2186,7 @@
       </c>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2215,6 +2207,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100054B99873F0D6546B559819D0825E003" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cffa56ad5792ecafcd3589bab1bbb308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xmlns:ns4="6c1397f4-a2e4-41e1-a56a-3ef30e67d471" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68c1c6e3f17b441c567360df559ac01a" ns3:_="" ns4:_="">
     <xsd:import namespace="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
@@ -2453,24 +2462,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA91FC1-FB23-421D-B0F5-8B5FD962DF28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2487,29 +2504,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: update cell label in updated criteria spreadsheet
OCD-4438
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
+++ b/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youngto\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE1997E-EF65-4C48-8976-553CBD4EBDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3AEC6B-33C0-4C07-BEF7-F47AC466149D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="1785" windowWidth="21600" windowHeight="11205" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="11" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>Standards Up-to-Date</t>
   </si>
   <si>
-    <t>Functionality Up-to-Date</t>
-  </si>
-  <si>
     <t>Code Sets Up-to-Date</t>
   </si>
   <si>
     <t>Total listings for criterion</t>
+  </si>
+  <si>
+    <t>Functionalities Tested Up-to-Date</t>
   </si>
 </sst>
 </file>
@@ -1876,11 +1876,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F5CA64-B349-4540-8897-9876CE15B639}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2021,7 +2023,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2062,7 +2064,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2146,7 +2148,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2207,23 +2209,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100054B99873F0D6546B559819D0825E003" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cffa56ad5792ecafcd3589bab1bbb308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xmlns:ns4="6c1397f4-a2e4-41e1-a56a-3ef30e67d471" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68c1c6e3f17b441c567360df559ac01a" ns3:_="" ns4:_="">
     <xsd:import namespace="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
@@ -2462,32 +2447,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA91FC1-FB23-421D-B0F5-8B5FD962DF28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2504,4 +2481,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: remove references to original workbook
OCD-4438
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
+++ b/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youngto\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3AEC6B-33C0-4C07-BEF7-F47AC466149D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB67B6C2-7E5D-4773-9C0C-6D7049D8F706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
@@ -194,15 +194,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fully Up-to-Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Fully Up-to-Date</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -314,15 +306,7 @@
           <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Requires Update</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Requires Update</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -452,15 +436,7 @@
           <c:idx val="6"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total listings for criterion</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Total listings for criterion</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -539,15 +515,7 @@
           <c:idx val="4"/>
           <c:order val="5"/>
           <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Code Sets Up-to-Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Code Sets Up-to-Date</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -623,15 +591,7 @@
           <c:idx val="5"/>
           <c:order val="6"/>
           <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Functionality Up-to-Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Functionality Up-to-Date</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -707,15 +667,7 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:strRef>
-              <c:f>[1]Template!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Standards Up-to-Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Standards Up-to-Date</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -806,21 +758,7 @@
                 <c:idx val="3"/>
                 <c:order val="3"/>
                 <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>[1]Template!$A$8</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>% Fully Up-to-Date</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
+                  <c:v>% Fully Up-to-Date</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
@@ -891,106 +829,88 @@
                   </c:extLst>
                 </c:dLbls>
                 <c:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>[1]Template!$B$6:$M$6</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
+                  <c:numLit>
+                    <c:formatCode>General</c:formatCode>
+                    <c:ptCount val="12"/>
+                    <c:pt idx="0">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="1">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="2">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="3">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="4">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="5">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="6">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="7">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="8">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="9">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="10">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="11">
+                      <c:v>0</c:v>
+                    </c:pt>
+                  </c:numLit>
                 </c:cat>
                 <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>[1]Template!$B$8:$M$8</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
+                  <c:numLit>
+                    <c:formatCode>General</c:formatCode>
+                    <c:ptCount val="12"/>
+                    <c:pt idx="0">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="1">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="2">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="3">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="4">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="5">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="6">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="7">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="8">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="9">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="10">
+                      <c:v>0</c:v>
+                    </c:pt>
+                    <c:pt idx="11">
+                      <c:v>0</c:v>
+                    </c:pt>
+                  </c:numLit>
                 </c:val>
                 <c:smooth val="0"/>
                 <c:extLst>
@@ -1005,21 +925,7 @@
                 <c:idx val="2"/>
                 <c:order val="4"/>
                 <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>[1]Template!$A$3</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Fully Up-to-Date</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
+                  <c:v>Fully Up-to-Date</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
@@ -1877,7 +1783,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,6 +2115,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100054B99873F0D6546B559819D0825E003" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cffa56ad5792ecafcd3589bab1bbb308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xmlns:ns4="6c1397f4-a2e4-41e1-a56a-3ef30e67d471" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68c1c6e3f17b441c567360df559ac01a" ns3:_="" ns4:_="">
     <xsd:import namespace="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
@@ -2447,24 +2370,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA91FC1-FB23-421D-B0F5-8B5FD962DF28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2481,29 +2412,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: make change to file to enusre it get's pushed to other envs.
OCD-4438
</commit_message>
<xml_diff>
--- a/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
+++ b/chpl/chpl-resources/src/main/resources/UpdatedCriteriaStatusReport.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youngto\workspaces\chpladmin\chpl-api\chpl\chpl-resources\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB67B6C2-7E5D-4773-9C0C-6D7049D8F706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C9C060-2115-4814-966F-30DE69EB4DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FE7958-BC57-49F5-AC1F-F5C1A57C91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="11" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1253,236 +1250,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Template"/>
-      <sheetName val="170.315 (a)(1)"/>
-      <sheetName val="170.315 (a)(2)"/>
-      <sheetName val="170.315 (a)(3)"/>
-      <sheetName val="170.315 (a)(4)"/>
-      <sheetName val="170.315 (a)(5)"/>
-      <sheetName val="170.315 (a)(9)"/>
-      <sheetName val="170.315 (a)(12)"/>
-      <sheetName val="170.315 (a)(14)"/>
-      <sheetName val="170.315 (a)(15)"/>
-      <sheetName val="170.315 (b)(2)"/>
-      <sheetName val="170.315 (b)(3)"/>
-      <sheetName val="170.315 (b)(7)"/>
-      <sheetName val="170.315 (b)(8)"/>
-      <sheetName val="170.315 (b)(9)"/>
-      <sheetName val="170.315 (b)(10)"/>
-      <sheetName val="170.315 (b)(11)"/>
-      <sheetName val="170.315 (c)(1)"/>
-      <sheetName val="170.315 (c)(2)"/>
-      <sheetName val="170.315 (c)(3)"/>
-      <sheetName val="170.315 (c)(4)"/>
-      <sheetName val="170.315 (d)(1)"/>
-      <sheetName val="170.315 (d)(2)"/>
-      <sheetName val="170.315 (d)(3)"/>
-      <sheetName val="170.315 (d)(4)"/>
-      <sheetName val="170.315 (d)(5)"/>
-      <sheetName val="170.315 (d)(6)"/>
-      <sheetName val="170.315 (d)(7)"/>
-      <sheetName val="170.315 (d)(8)"/>
-      <sheetName val="170.315 (d)(9)"/>
-      <sheetName val="170.315 (d)(10)"/>
-      <sheetName val="170.315 (d)(11)"/>
-      <sheetName val="170.315 (d)(12)"/>
-      <sheetName val="170.315 (d)(13)"/>
-      <sheetName val="170.315 (e)(1)"/>
-      <sheetName val="170.315 (e)(3)"/>
-      <sheetName val="170.315 (f)(1)"/>
-      <sheetName val="170.315 (f)(2)"/>
-      <sheetName val="170.315 (f)(3)"/>
-      <sheetName val="170.315 (f)(4)"/>
-      <sheetName val="170.315 (f)(5)"/>
-      <sheetName val="170.315 (f)(6)"/>
-      <sheetName val="170.315 (f)(7)"/>
-      <sheetName val="170.315 (g)(1)"/>
-      <sheetName val="170.315 (g)(2)"/>
-      <sheetName val="170.315 (g)(3)"/>
-      <sheetName val="170.315 (g)(4)"/>
-      <sheetName val="170.315 (g)(5)"/>
-      <sheetName val="170.315 (g)(6)"/>
-      <sheetName val="170.315 (g)(7)"/>
-      <sheetName val="170.315 (g)(9)"/>
-      <sheetName val="170.315 (g)(10)"/>
-      <sheetName val="170.315 (h)(1)"/>
-      <sheetName val="170.315 (h)(2)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Requires Update</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Fully Up-to-Date</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Code Sets Up-to-Date</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Functionality Up-to-Date</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Standards Up-to-Date</v>
-          </cell>
-          <cell r="B6">
-            <v>0</v>
-          </cell>
-          <cell r="C6">
-            <v>0</v>
-          </cell>
-          <cell r="D6">
-            <v>0</v>
-          </cell>
-          <cell r="E6">
-            <v>0</v>
-          </cell>
-          <cell r="F6">
-            <v>0</v>
-          </cell>
-          <cell r="G6">
-            <v>0</v>
-          </cell>
-          <cell r="H6">
-            <v>0</v>
-          </cell>
-          <cell r="I6">
-            <v>0</v>
-          </cell>
-          <cell r="J6">
-            <v>0</v>
-          </cell>
-          <cell r="K6">
-            <v>0</v>
-          </cell>
-          <cell r="L6">
-            <v>0</v>
-          </cell>
-          <cell r="M6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Total listings for criterion</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>% Fully Up-to-Date</v>
-          </cell>
-          <cell r="B8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="C8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="D8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="E8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="F8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="G8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="H8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="I8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="J8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="K8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="L8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-          <cell r="M8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1783,7 +1550,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,23 +1882,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100054B99873F0D6546B559819D0825E003" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cffa56ad5792ecafcd3589bab1bbb308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xmlns:ns4="6c1397f4-a2e4-41e1-a56a-3ef30e67d471" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68c1c6e3f17b441c567360df559ac01a" ns3:_="" ns4:_="">
     <xsd:import namespace="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
@@ -2370,32 +2120,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="63b9e3fc-e3d9-4b25-9f08-bf71a160189f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBA91FC1-FB23-421D-B0F5-8B5FD962DF28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2412,4 +2154,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30F5C5E2-FF74-4F0D-A48F-2A211F06009F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5AE281-2091-44EB-95A1-2B115BF9F717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6c1397f4-a2e4-41e1-a56a-3ef30e67d471"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="63b9e3fc-e3d9-4b25-9f08-bf71a160189f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>